<commit_message>
-- added structure of project
</commit_message>
<xml_diff>
--- a/helpful-information/tinder-db-structure.xlsx
+++ b/helpful-information/tinder-db-structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Efqan\Desktop\IBA_Tech_Academy_Lessons\step-project-tinder\helpful-information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939D682D-6EF3-4F37-A673-CFC2EE6EE878}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E810F4-B79A-43E5-A760-3A248244C56F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F4AC15F5-D98F-471B-A378-D9493762402D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F4AC15F5-D98F-471B-A378-D9493762402D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,8 +153,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{79100238-CA93-4E57-92E2-DF57C03CA2FA}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -466,7 +494,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J6" sqref="J6:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>